<commit_message>
Change exception color coding to grayscale
Updated exception table colors from green/blue/red to grayscale:
- Available now: Light gray (#e0e0e0)
- Currently allocated: Medium gray (#c0c0c0)
- Over-allocated: Dark gray (#a0a0a0)
- Vacation: White (unchanged)

Co-Authored-By: Claude Sonnet 4.5 <noreply@anthropic.com>
</commit_message>
<xml_diff>
--- a/data/projects.xlsx
+++ b/data/projects.xlsx
@@ -404,7 +404,7 @@
   <cols>
     <col min="1" max="1" width="10.83203125" customWidth="1"/>
     <col min="2" max="2" width="40.83203125" customWidth="1"/>
-    <col min="3" max="3" width="10.83203125" customWidth="1"/>
+    <col min="3" max="3" width="40.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -415,7 +415,7 @@
         <v>Name</v>
       </c>
       <c r="C1" t="str">
-        <v>ClientID</v>
+        <v>Client</v>
       </c>
     </row>
     <row r="2">

</xml_diff>